<commit_message>
made endpoint for intro text
</commit_message>
<xml_diff>
--- a/data/excel_dumps/patients/patient_1.xlsx
+++ b/data/excel_dumps/patients/patient_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Student Id</t>
   </si>
@@ -38,7 +38,19 @@
     <t>false</t>
   </si>
   <si>
-    <t>2019-10-21</t>
+    <t>2019-11-04</t>
+  </si>
+  <si>
+    <t>chaotsai@stonybrook.edu</t>
+  </si>
+  <si>
+    <t>2019-12-01</t>
+  </si>
+  <si>
+    <t>2019-12-03</t>
+  </si>
+  <si>
+    <t>vlgarcia@stonybrook.edu</t>
   </si>
 </sst>
 </file>
@@ -377,7 +389,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,7 +425,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -430,7 +442,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -447,10 +459,95 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>